<commit_message>
moved the CanMove from each chesspiece subclass up to the main ChessPiece class. All pieces move properly. need to begin implementation of taking turns, showing fallen pieces, implement pawns turning into queens ect.
</commit_message>
<xml_diff>
--- a/ChessMoves.xlsx
+++ b/ChessMoves.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a5d26c7373c3f512/Documents/GitHub/csci-325-spring-2017_FinalProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mille\OneDrive\Documents\GitHub\csci-325-spring-2017_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>up</t>
   </si>
@@ -75,6 +75,83 @@
   </si>
   <si>
     <t>move is always dest minus origin</t>
+  </si>
+  <si>
+    <t>COMPAS { SO,SW, WE, NW, NO, NE, EA, SE }</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>WE</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>D1 - O1 &lt; 0</t>
+  </si>
+  <si>
+    <t>D1 - O1 &gt; 0</t>
+  </si>
+  <si>
+    <t>D0 - O0 == 0</t>
+  </si>
+  <si>
+    <t>D1 - O1 == 0</t>
+  </si>
+  <si>
+    <t>D0 - O0 &gt; 0</t>
+  </si>
+  <si>
+    <t>D0 - O0 &lt; 0</t>
+  </si>
+  <si>
+    <t>if ( compas == NO ) { D0 - O0 == 0;
+D1 - O1 &gt; 0;}</t>
+  </si>
+  <si>
+    <t>if ( compas == NW ) { D0 - O0 &lt; 0;
+D1 - O1 &gt; 0;}</t>
+  </si>
+  <si>
+    <t>if ( compas == WE ) { D0 - O0 &lt; 0;
+D1 - O1 == 0;}</t>
+  </si>
+  <si>
+    <t>if ( compas == SW ) { D0 - O0 &lt; 0;
+D1 - O1 &lt; 0;}</t>
+  </si>
+  <si>
+    <t>if ( compas == SO ) { D0 - O0 == 0;
+D1 - O1 &lt; 0;}</t>
+  </si>
+  <si>
+    <t>if ( compas == NE ) { D0 - O0 &gt; 0;
+D1 - O1 &gt; 0;}</t>
+  </si>
+  <si>
+    <t>if ( compas == EA ) { D0 - O0 &gt; 0;
+D1 - O1 == 0;}</t>
+  </si>
+  <si>
+    <t>if ( compas == SE ) { D0 - O0 &gt; 0;
+D1 - O1 &lt; 0;}</t>
   </si>
 </sst>
 </file>
@@ -154,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -190,6 +267,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -507,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AE14"/>
+  <dimension ref="B2:AJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30:V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -539,6 +619,8 @@
     <col min="28" max="28" width="4.52734375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="3.41015625" customWidth="1"/>
     <col min="30" max="30" width="4.9375" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="10.3515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.3515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:31" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -753,10 +835,10 @@
         <v>5</v>
       </c>
       <c r="X5" s="16"/>
-      <c r="Z5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="5"/>
+      <c r="Z5" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="17"/>
       <c r="AC5" s="15" t="s">
         <v>5</v>
       </c>
@@ -887,10 +969,10 @@
       <c r="T7" s="3">
         <v>3</v>
       </c>
-      <c r="Z7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="5"/>
+      <c r="Z7" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="17"/>
     </row>
     <row r="8" spans="2:31" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D8">
@@ -1111,25 +1193,298 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:31" ht="79.349999999999994" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:31" ht="34" customHeight="1" x14ac:dyDescent="0.5">
       <c r="E12" s="2"/>
       <c r="F12"/>
-      <c r="W12" s="17" t="s">
+      <c r="W12" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="X12" s="17"/>
-      <c r="Y12" s="17"/>
-      <c r="AC12" s="17"/>
-      <c r="AD12" s="17"/>
-      <c r="AE12" s="17"/>
-    </row>
-    <row r="13" spans="2:31" ht="60.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="W13" s="17"/>
-      <c r="X13" s="17"/>
-      <c r="Y13" s="17"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="18"/>
+      <c r="AC12" s="18"/>
+      <c r="AD12" s="18"/>
+      <c r="AE12" s="18"/>
+    </row>
+    <row r="13" spans="2:31" x14ac:dyDescent="0.5">
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.5">
       <c r="F14"/>
+      <c r="H14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:31" x14ac:dyDescent="0.5">
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15" s="2">
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <v>5</v>
+      </c>
+      <c r="N15" s="2">
+        <v>6</v>
+      </c>
+      <c r="O15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="M17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V17" t="str">
+        <f>"if (" &amp; AG17 &amp; " &amp;&amp; " &amp; AH17 &amp; ") { comp = " &amp; M17 &amp; ";}"</f>
+        <v>if (D0 - O0 == 0 &amp;&amp; D1 - O1 &gt; 0) { comp = NO;}</v>
+      </c>
+      <c r="AE17" s="2"/>
+      <c r="AG17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="K18" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="O18" t="s">
+        <v>23</v>
+      </c>
+      <c r="V18" t="str">
+        <f>"if (" &amp; AE18 &amp; " &amp;&amp; " &amp; AF18 &amp; ") { comp = " &amp; K18 &amp; ";}"</f>
+        <v>if (D0 - O0 &lt; 0 &amp;&amp; D1 - O1 &gt; 0) { comp = NW;}</v>
+      </c>
+      <c r="Z18" t="str">
+        <f>"if (" &amp; AI18 &amp; " &amp;&amp; " &amp; AJ18 &amp; ") { comp = " &amp; O18 &amp; ";}"</f>
+        <v>if (D0 - O0 &gt; 0 &amp;&amp; D1 - O1 &gt; 0) { comp = NE;}</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="K19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="O19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V19" t="str">
+        <f t="shared" ref="V19:V20" si="0">"if (" &amp; AE19 &amp; " &amp;&amp; " &amp; AF19 &amp; ") { comp = " &amp; K19 &amp; ";}"</f>
+        <v>if (D0 - O0 &lt; 0 &amp;&amp; D1 - O1 == 0) { comp = WE;}</v>
+      </c>
+      <c r="Z19" t="str">
+        <f t="shared" ref="Z19:Z20" si="1">"if (" &amp; AI19 &amp; " &amp;&amp; " &amp; AJ19 &amp; ") { comp = " &amp; O19 &amp; ";}"</f>
+        <v>if (D0 - O0 &gt; 0 &amp;&amp; D1 - O1 == 0) { comp = EA;}</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="K20" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="O20" t="s">
+        <v>25</v>
+      </c>
+      <c r="V20" t="str">
+        <f t="shared" si="0"/>
+        <v>if (D0 - O0 &lt; 0 &amp;&amp; D1 - O1 &lt; 0) { comp = SW;}</v>
+      </c>
+      <c r="Z20" t="str">
+        <f t="shared" si="1"/>
+        <v>if (D0 - O0 &gt; 0 &amp;&amp; D1 - O1 &lt; 0) { comp = SE;}</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="M21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V21" t="str">
+        <f>"if (" &amp; AG21 &amp; " &amp;&amp; " &amp; AH21 &amp; ") { comp = " &amp; M21 &amp; ";}"</f>
+        <v>if (D0 - O0 == 0 &amp;&amp; D1 - O1 &lt; 0) { comp = SO;}</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="Z23" s="5"/>
+    </row>
+    <row r="24" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="V24" t="str">
+        <f>"if ( compas == " &amp; M17 &amp; " ) { " &amp; AG17  &amp; ";
+" &amp; AH17 &amp; ";}"</f>
+        <v>if ( compas == NO ) { D0 - O0 == 0;
+D1 - O1 &gt; 0;}</v>
+      </c>
+      <c r="Z24"/>
+    </row>
+    <row r="25" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="V25" t="str">
+        <f>"if ( compas == " &amp; K18 &amp; " ) { " &amp; AE18  &amp; ";
+" &amp; AF18 &amp; ";}"</f>
+        <v>if ( compas == NW ) { D0 - O0 &lt; 0;
+D1 - O1 &gt; 0;}</v>
+      </c>
+      <c r="Z25" t="str">
+        <f>"if ( compas == " &amp; O18 &amp; " ) { " &amp; AI18  &amp; ";
+" &amp; AJ18 &amp; ";}"</f>
+        <v>if ( compas == NE ) { D0 - O0 &gt; 0;
+D1 - O1 &gt; 0;}</v>
+      </c>
+    </row>
+    <row r="26" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="V26" t="str">
+        <f>"if ( compas == " &amp; K19 &amp; " ) { " &amp; AE19  &amp; ";
+" &amp; AF19 &amp; ";}"</f>
+        <v>if ( compas == WE ) { D0 - O0 &lt; 0;
+D1 - O1 == 0;}</v>
+      </c>
+      <c r="Z26" t="str">
+        <f>"if ( compas == " &amp; O19 &amp; " ) { " &amp; AI19  &amp; ";
+" &amp; AJ19 &amp; ";}"</f>
+        <v>if ( compas == EA ) { D0 - O0 &gt; 0;
+D1 - O1 == 0;}</v>
+      </c>
+    </row>
+    <row r="27" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="V27" t="str">
+        <f>"if ( compas == " &amp; K20 &amp; " ) { " &amp; AE20  &amp; ";
+" &amp; AF20 &amp; ";}"</f>
+        <v>if ( compas == SW ) { D0 - O0 &lt; 0;
+D1 - O1 &lt; 0;}</v>
+      </c>
+      <c r="Z27" t="str">
+        <f>"if ( compas == " &amp; O20 &amp; " ) { " &amp; AI20  &amp; ";
+" &amp; AJ20 &amp; ";}"</f>
+        <v>if ( compas == SE ) { D0 - O0 &gt; 0;
+D1 - O1 &lt; 0;}</v>
+      </c>
+    </row>
+    <row r="28" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="V28" t="str">
+        <f>"if ( compas == " &amp; M21 &amp; " ) { " &amp; AG21  &amp; ";
+" &amp; AH21 &amp; ";}"</f>
+        <v>if ( compas == SO ) { D0 - O0 == 0;
+D1 - O1 &lt; 0;}</v>
+      </c>
+    </row>
+    <row r="30" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="V30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="V31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="11:36" x14ac:dyDescent="0.5">
+      <c r="V32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="22:22" x14ac:dyDescent="0.5">
+      <c r="V33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="22:22" x14ac:dyDescent="0.5">
+      <c r="V34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="22:22" x14ac:dyDescent="0.5">
+      <c r="V35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="22:22" x14ac:dyDescent="0.5">
+      <c r="V36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="22:22" x14ac:dyDescent="0.5">
+      <c r="V37" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1140,5 +1495,6 @@
     <mergeCell ref="W13:Y13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>